<commit_message>
update excel and upload source files
</commit_message>
<xml_diff>
--- a/data/ruv_risks.xlsx
+++ b/data/ruv_risks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOME\Desktop\CDS\ruv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB900F49-040A-4007-80CD-6AB6558E22DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C707E8-CCF9-416C-A5D7-F5075B87314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{567DBFD7-7C79-42B9-A598-9C93525BF770}"/>
+    <workbookView xWindow="28680" yWindow="-12600" windowWidth="29040" windowHeight="15840" xr2:uid="{567DBFD7-7C79-42B9-A598-9C93525BF770}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>risk_de</t>
   </si>
@@ -233,6 +233,21 @@
   </si>
   <si>
     <t>Langzeitvergleich 1992 bis 2022</t>
+  </si>
+  <si>
+    <t>Hinterherhinken bei Digitalisierung</t>
+  </si>
+  <si>
+    <t>Zerbrechen der Partnerschaft</t>
+  </si>
+  <si>
+    <t>häufiger Pandemien durch Globalisierung</t>
+  </si>
+  <si>
+    <t>Grafiken zur Studie 2013</t>
+  </si>
+  <si>
+    <t>https://www.rosenheim24.de/deutschland/aengste-deutschen-2013-grafiken-studie-infocenters-rvversicherung-3094771.html</t>
   </si>
 </sst>
 </file>
@@ -595,16 +610,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFFFB71-7D65-4269-AE0C-65B728FE8B6F}">
-  <dimension ref="A1:AF27"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.44140625" customWidth="1"/>
-    <col min="2" max="19" width="8.88671875" customWidth="1"/>
+    <col min="2" max="21" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
@@ -923,6 +938,18 @@
       <c r="J4">
         <v>44</v>
       </c>
+      <c r="U4">
+        <v>42</v>
+      </c>
+      <c r="V4">
+        <v>41</v>
+      </c>
+      <c r="W4">
+        <v>42</v>
+      </c>
+      <c r="X4">
+        <v>43</v>
+      </c>
       <c r="Y4">
         <v>49</v>
       </c>
@@ -1157,6 +1184,33 @@
       <c r="E7">
         <v>35</v>
       </c>
+      <c r="U7">
+        <v>39</v>
+      </c>
+      <c r="V7">
+        <v>40</v>
+      </c>
+      <c r="W7">
+        <v>40</v>
+      </c>
+      <c r="X7">
+        <v>38</v>
+      </c>
+      <c r="Y7">
+        <v>37</v>
+      </c>
+      <c r="Z7">
+        <v>46</v>
+      </c>
+      <c r="AD7">
+        <v>32</v>
+      </c>
+      <c r="AE7">
+        <v>35</v>
+      </c>
+      <c r="AF7">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1168,6 +1222,24 @@
       <c r="D8">
         <v>33</v>
       </c>
+      <c r="U8">
+        <v>31</v>
+      </c>
+      <c r="V8">
+        <v>29</v>
+      </c>
+      <c r="W8">
+        <v>31</v>
+      </c>
+      <c r="X8">
+        <v>28</v>
+      </c>
+      <c r="Y8">
+        <v>27</v>
+      </c>
+      <c r="Z8">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1277,6 +1349,30 @@
       <c r="H10">
         <v>47</v>
       </c>
+      <c r="U10">
+        <v>38</v>
+      </c>
+      <c r="V10">
+        <v>34</v>
+      </c>
+      <c r="W10">
+        <v>35</v>
+      </c>
+      <c r="X10">
+        <v>32</v>
+      </c>
+      <c r="Y10">
+        <v>31</v>
+      </c>
+      <c r="Z10">
+        <v>36</v>
+      </c>
+      <c r="AD10">
+        <v>24</v>
+      </c>
+      <c r="AE10">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1900,6 +1996,9 @@
       <c r="Y20">
         <v>49</v>
       </c>
+      <c r="Z20">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -2099,6 +2198,51 @@
       </c>
       <c r="AF27">
         <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="U29">
+        <v>18</v>
+      </c>
+      <c r="V29">
+        <v>16</v>
+      </c>
+      <c r="W29">
+        <v>20</v>
+      </c>
+      <c r="X29">
+        <v>18</v>
+      </c>
+      <c r="Y29">
+        <v>15</v>
+      </c>
+      <c r="Z29">
+        <v>21</v>
+      </c>
+      <c r="AD29">
+        <v>10</v>
+      </c>
+      <c r="AE29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD30">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2112,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBD267D-AA93-40B9-A852-3EE57CFA1433}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2428,8 +2572,14 @@
       <c r="B28">
         <v>2018</v>
       </c>
+      <c r="C28" s="1">
+        <v>43259</v>
+      </c>
+      <c r="D28" s="1">
+        <v>43664</v>
+      </c>
       <c r="E28">
-        <v>2400</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2439,8 +2589,14 @@
       <c r="B29">
         <v>2019</v>
       </c>
+      <c r="C29" s="1">
+        <v>43598</v>
+      </c>
+      <c r="D29" s="1">
+        <v>43669</v>
+      </c>
       <c r="E29">
-        <v>2400</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2450,6 +2606,12 @@
       <c r="B30">
         <v>2020</v>
       </c>
+      <c r="C30" s="1">
+        <v>43990</v>
+      </c>
+      <c r="D30" s="1">
+        <v>44033</v>
+      </c>
       <c r="E30">
         <v>2400</v>
       </c>
@@ -2460,6 +2622,12 @@
       </c>
       <c r="B31">
         <v>2021</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44341</v>
+      </c>
+      <c r="D31" s="1">
+        <v>44381</v>
       </c>
       <c r="E31">
         <v>2400</v>
@@ -2490,10 +2658,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264B4649-857F-4680-ABCE-F216D3A9D4F7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2509,6 +2677,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update excel and rerun r file
</commit_message>
<xml_diff>
--- a/data/ruv_risks.xlsx
+++ b/data/ruv_risks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOME\Desktop\CDS\ruv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBED462C-97FB-4E31-ACB1-1712C6BA14DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C17CB6E-9BAD-483F-BFCA-4D8524C9EEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12600" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{567DBFD7-7C79-42B9-A598-9C93525BF770}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{567DBFD7-7C79-42B9-A598-9C93525BF770}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
   <si>
     <t>risk_de</t>
   </si>
@@ -250,7 +250,16 @@
     <t>https://www.rosenheim24.de/deutschland/aengste-deutschen-2013-grafiken-studie-infocenters-rvversicherung-3094771.html</t>
   </si>
   <si>
-    <t>fehlender Bürgernähe der Politiker</t>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>item wording changed from "fehlender Bürgernähe der Politiker" to "Überforderung der Politiker" possibly from w16 onwards.</t>
+  </si>
+  <si>
+    <t>item wording changed to included "Wetterextreme" in later waves, unclear which wave exactly. Possible overlap with Klimawandel.</t>
+  </si>
+  <si>
+    <t>inclusion of "Corona-Infektion" from w29 onwards.</t>
   </si>
 </sst>
 </file>
@@ -613,164 +622,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFFFB71-7D65-4269-AE0C-65B728FE8B6F}">
-  <dimension ref="A1:AF31"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.44140625" customWidth="1"/>
-    <col min="2" max="21" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="22" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="2">
         <v>48</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>53</v>
-      </c>
-      <c r="D2">
-        <v>52</v>
       </c>
       <c r="E2">
         <v>52</v>
       </c>
       <c r="F2">
+        <v>52</v>
+      </c>
+      <c r="G2">
         <v>53</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>55</v>
-      </c>
-      <c r="H2">
-        <v>48</v>
       </c>
       <c r="I2">
         <v>48</v>
       </c>
       <c r="J2">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K2">
         <v>54</v>
       </c>
       <c r="L2">
+        <v>54</v>
+      </c>
+      <c r="M2">
         <v>51</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>55</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>52</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>64</v>
-      </c>
-      <c r="P2">
-        <v>51</v>
       </c>
       <c r="Q2">
         <v>51</v>
@@ -779,369 +792,369 @@
         <v>51</v>
       </c>
       <c r="S2">
+        <v>51</v>
+      </c>
+      <c r="T2">
         <v>49</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>57</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>50</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>46</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>49</v>
-      </c>
-      <c r="X2">
-        <v>47</v>
       </c>
       <c r="Y2">
         <v>47</v>
       </c>
       <c r="Z2">
+        <v>47</v>
+      </c>
+      <c r="AA2">
         <v>55</v>
-      </c>
-      <c r="AA2">
-        <v>47</v>
       </c>
       <c r="AB2">
         <v>47</v>
       </c>
       <c r="AC2">
+        <v>47</v>
+      </c>
+      <c r="AD2">
         <v>35</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>32</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>35</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>47</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>53</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>49</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>48</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>52</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>57</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>50</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>52</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>55</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>53</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>54</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>57</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>55</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>62</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>52</v>
-      </c>
-      <c r="Q3">
-        <v>53</v>
       </c>
       <c r="R3">
         <v>53</v>
       </c>
       <c r="S3">
+        <v>53</v>
+      </c>
+      <c r="T3">
         <v>54</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>61</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>55</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>50</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>55</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>51</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>49</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>57</v>
-      </c>
-      <c r="AA3">
-        <v>52</v>
       </c>
       <c r="AB3">
         <v>52</v>
       </c>
       <c r="AC3">
+        <v>52</v>
+      </c>
+      <c r="AD3">
         <v>45</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>41</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>43</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>46</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>48</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>50</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>49</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>53</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>44</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>45</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>41</v>
-      </c>
-      <c r="R4">
-        <v>37</v>
       </c>
       <c r="S4">
         <v>37</v>
       </c>
       <c r="T4">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="U4">
         <v>42</v>
       </c>
       <c r="V4">
+        <v>42</v>
+      </c>
+      <c r="W4">
         <v>41</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>42</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>43</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>49</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>67</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>61</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>63</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>55</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>43</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>42</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <v>40</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>45</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>40</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>42</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>44</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>43</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>38</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>36</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>40</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>36</v>
-      </c>
-      <c r="L5">
-        <v>33</v>
       </c>
       <c r="M5">
         <v>33</v>
       </c>
       <c r="N5">
+        <v>33</v>
+      </c>
+      <c r="O5">
         <v>29</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>24</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>25</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>28</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>25</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>24</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>29</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>28</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>22</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>24</v>
-      </c>
-      <c r="X5">
-        <v>26</v>
       </c>
       <c r="Y5">
         <v>26</v>
       </c>
       <c r="Z5">
+        <v>26</v>
+      </c>
+      <c r="AA5">
         <v>30</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>29</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>28</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>23</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>18</v>
-      </c>
-      <c r="AE5">
-        <v>19</v>
       </c>
       <c r="AF5">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="2">
         <v>37</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>44</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>46</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>51</v>
-      </c>
-      <c r="G6">
-        <v>52</v>
       </c>
       <c r="H6">
         <v>52</v>
       </c>
       <c r="I6">
+        <v>52</v>
+      </c>
+      <c r="J6">
         <v>48</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>44</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>46</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>44</v>
-      </c>
-      <c r="M6">
-        <v>53</v>
       </c>
       <c r="N6">
         <v>53</v>
       </c>
       <c r="O6">
+        <v>53</v>
+      </c>
+      <c r="P6">
         <v>65</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>51</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>47</v>
-      </c>
-      <c r="R6">
-        <v>48</v>
       </c>
       <c r="S6">
         <v>48</v>
@@ -1150,1227 +1163,1226 @@
         <v>48</v>
       </c>
       <c r="U6">
+        <v>48</v>
+      </c>
+      <c r="V6">
         <v>36</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>32</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>36</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>33</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>32</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>38</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>27</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>25</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>24</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>25</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>24</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="2">
         <v>33</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>41</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>36</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>35</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>48</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>38</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>41</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>37</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>47</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>39</v>
-      </c>
-      <c r="V7">
-        <v>40</v>
       </c>
       <c r="W7">
         <v>40</v>
       </c>
       <c r="X7">
+        <v>40</v>
+      </c>
+      <c r="Y7">
         <v>38</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>37</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>46</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>37</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>39</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>34</v>
       </c>
-      <c r="AD7">
+      <c r="AE7">
         <v>32</v>
       </c>
-      <c r="AE7">
+      <c r="AF7">
         <v>35</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="2">
         <v>33</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>33</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>40</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>30</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>31</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>30</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>36</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>31</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>29</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>31</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>28</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>27</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="2">
         <v>29</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>57</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>47</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>46</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>65</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>60</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>58</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>54</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>57</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>63</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>62</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>67</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>66</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>72</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>70</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>66</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>76</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>63</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>68</v>
-      </c>
-      <c r="U9">
-        <v>63</v>
       </c>
       <c r="V9">
         <v>63</v>
       </c>
       <c r="W9">
+        <v>63</v>
+      </c>
+      <c r="X9">
         <v>61</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>58</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>48</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>54</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>50</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>49</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>43</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>51</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>50</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>36</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>47</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>48</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>43</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>42</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>34</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>46</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>38</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>34</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>35</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>32</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>31</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>36</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>28</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>27</v>
-      </c>
-      <c r="AC10">
-        <v>24</v>
       </c>
       <c r="AD10">
         <v>24</v>
       </c>
       <c r="AE10">
+        <v>24</v>
+      </c>
+      <c r="AF10">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>65</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>67</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>65</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>55</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>45</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>48</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>53</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>66</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>64</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>68</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>61</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>45</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>47</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>65</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>61</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>37</v>
-      </c>
-      <c r="V11">
-        <v>39</v>
       </c>
       <c r="W11">
         <v>39</v>
       </c>
       <c r="X11">
+        <v>39</v>
+      </c>
+      <c r="Y11">
         <v>33</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>31</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>43</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>26</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>29</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>28</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>40</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>31</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C12" s="2">
         <v>32</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>39</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>26</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>34</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>31</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>32</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>24</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>60</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>28</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>27</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>34</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>44</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>39</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>33</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>31</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>36</v>
-      </c>
-      <c r="R12">
-        <v>31</v>
       </c>
       <c r="S12">
         <v>31</v>
       </c>
       <c r="T12">
+        <v>31</v>
+      </c>
+      <c r="U12">
         <v>42</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>40</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>29</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>32</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>35</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>41</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>54</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>46</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>35</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>24</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>19</v>
       </c>
-      <c r="AE12">
+      <c r="AF12">
         <v>16</v>
       </c>
-      <c r="AF12">
+      <c r="AG12">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>51</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>48</v>
-      </c>
-      <c r="K13">
-        <v>57</v>
       </c>
       <c r="L13">
         <v>57</v>
       </c>
       <c r="M13">
+        <v>57</v>
+      </c>
+      <c r="N13">
         <v>68</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>65</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>70</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>60</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>48</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>58</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>66</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>67</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>48</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>52</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>50</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>41</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>40</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>52</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>37</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>39</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>35</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>48</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>40</v>
       </c>
-      <c r="AF13">
+      <c r="AG13">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="K14">
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14">
         <v>48</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>54</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>66</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>59</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>64</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>63</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>51</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>49</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>53</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>62</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>53</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>55</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>45</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>44</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>48</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>65</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>55</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>61</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>47</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>40</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>41</v>
       </c>
-      <c r="AF14">
+      <c r="AG14">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>52</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>30</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>25</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>23</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>25</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>24</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>21</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>36</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>58</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>57</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>43</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>41</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>50</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>41</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>46</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>53</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>50</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>39</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>43</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>39</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>52</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>73</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>71</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <v>59</v>
       </c>
-      <c r="AC15">
+      <c r="AD15">
         <v>44</v>
       </c>
-      <c r="AD15">
+      <c r="AE15">
         <v>35</v>
       </c>
-      <c r="AE15">
+      <c r="AF15">
         <v>32</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="M16">
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16">
         <v>55</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>56</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>49</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>52</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>59</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>58</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>56</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>64</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>60</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>52</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>56</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>51</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>53</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>52</v>
-      </c>
-      <c r="AA16">
-        <v>56</v>
       </c>
       <c r="AB16">
         <v>56</v>
       </c>
       <c r="AC16">
+        <v>56</v>
+      </c>
+      <c r="AD16">
         <v>41</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>44</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>41</v>
       </c>
-      <c r="AF16">
+      <c r="AG16">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>48</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>41</v>
-      </c>
-      <c r="AD17">
-        <v>40</v>
       </c>
       <c r="AE17">
         <v>40</v>
       </c>
       <c r="AF17">
+        <v>40</v>
+      </c>
+      <c r="AG17">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>56</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>52</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>46</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>48</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>51</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>50</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>52</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>64</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>70</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>57</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>54</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>56</v>
-      </c>
-      <c r="Y18">
-        <v>57</v>
       </c>
       <c r="Z18">
         <v>57</v>
       </c>
       <c r="AA18">
+        <v>57</v>
+      </c>
+      <c r="AB18">
         <v>58</v>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <v>55</v>
-      </c>
-      <c r="AC18">
-        <v>42</v>
       </c>
       <c r="AD18">
         <v>42</v>
       </c>
       <c r="AE18">
+        <v>42</v>
+      </c>
+      <c r="AF18">
         <v>43</v>
       </c>
-      <c r="AF18">
+      <c r="AG18">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>70</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>73</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>68</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>60</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>64</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>65</v>
-      </c>
-      <c r="AA19">
-        <v>58</v>
       </c>
       <c r="AB19">
         <v>58</v>
       </c>
       <c r="AC19">
+        <v>58</v>
+      </c>
+      <c r="AD19">
         <v>44</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>49</v>
       </c>
-      <c r="AE19">
+      <c r="AF19">
         <v>50</v>
       </c>
-      <c r="AF19">
+      <c r="AG19">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>60</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>65</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>53</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>45</v>
-      </c>
-      <c r="Y20">
-        <v>49</v>
       </c>
       <c r="Z20">
         <v>49</v>
       </c>
       <c r="AA20">
+        <v>49</v>
+      </c>
+      <c r="AB20">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>50</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>66</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>57</v>
       </c>
-      <c r="AB21">
+      <c r="AC21">
         <v>61</v>
       </c>
-      <c r="AC21">
+      <c r="AD21">
         <v>56</v>
       </c>
-      <c r="AD21">
+      <c r="AE21">
         <v>43</v>
-      </c>
-      <c r="AE21">
-        <v>45</v>
       </c>
       <c r="AF21">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>45</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>44</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>51</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>52</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>43</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>48</v>
-      </c>
-      <c r="L22">
-        <v>45</v>
       </c>
       <c r="M22">
         <v>45</v>
       </c>
       <c r="N22">
+        <v>45</v>
+      </c>
+      <c r="O22">
         <v>42</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>46</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>42</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>44</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>40</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>39</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>47</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>40</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>43</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>40</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>42</v>
       </c>
-      <c r="Y22">
+      <c r="Z22">
         <v>49</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>68</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <v>62</v>
       </c>
-      <c r="AB22">
+      <c r="AC22">
         <v>57</v>
       </c>
-      <c r="AC22">
+      <c r="AD22">
         <v>47</v>
       </c>
-      <c r="AD22">
+      <c r="AE22">
         <v>37</v>
       </c>
-      <c r="AE22">
+      <c r="AF22">
         <v>38</v>
       </c>
-      <c r="AF22">
+      <c r="AG22">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AB23">
+      <c r="B23" s="3"/>
+      <c r="AC23">
         <v>69</v>
       </c>
-      <c r="AC23">
+      <c r="AD23">
         <v>55</v>
       </c>
-      <c r="AD23">
+      <c r="AE23">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="AC24">
+      <c r="AD24">
         <v>45</v>
       </c>
-      <c r="AF24">
+      <c r="AG24">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>61</v>
       </c>
-      <c r="AE25">
+      <c r="AF25">
         <v>53</v>
       </c>
-      <c r="AF25">
+      <c r="AG25">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>62</v>
       </c>
-      <c r="AF26">
+      <c r="AG26">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>64</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>54</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>43</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>41</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <v>38</v>
       </c>
-      <c r="Y27">
+      <c r="Z27">
         <v>37</v>
       </c>
-      <c r="Z27">
+      <c r="AA27">
         <v>46</v>
       </c>
-      <c r="AA27">
+      <c r="AB27">
         <v>42</v>
       </c>
-      <c r="AB27">
+      <c r="AC27">
         <v>40</v>
       </c>
-      <c r="AC27">
+      <c r="AD27">
         <v>32</v>
       </c>
-      <c r="AD27">
+      <c r="AE27">
         <v>25</v>
-      </c>
-      <c r="AE27">
-        <v>30</v>
       </c>
       <c r="AF27">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>66</v>
       </c>
-      <c r="AE28">
+      <c r="AF28">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>24</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <v>18</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>19</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <v>21</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>16</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>23</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>18</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>16</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>20</v>
       </c>
-      <c r="X29">
+      <c r="Y29">
         <v>18</v>
       </c>
-      <c r="Y29">
+      <c r="Z29">
         <v>15</v>
       </c>
-      <c r="Z29">
+      <c r="AA29">
         <v>21</v>
       </c>
-      <c r="AA29">
+      <c r="AB29">
         <v>17</v>
-      </c>
-      <c r="AB29">
-        <v>18</v>
       </c>
       <c r="AC29">
         <v>18</v>
       </c>
       <c r="AD29">
+        <v>18</v>
+      </c>
+      <c r="AE29">
         <v>10</v>
       </c>
-      <c r="AE29">
+      <c r="AF29">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>68</v>
       </c>
-      <c r="AD30">
+      <c r="AE30">
         <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>71</v>
-      </c>
-      <c r="O31">
-        <v>64</v>
-      </c>
-      <c r="P31">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2384,7 +2396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBD267D-AA93-40B9-A852-3EE57CFA1433}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>

</xml_diff>